<commit_message>
fix: Agregar cohorte para produccion de ARL
</commit_message>
<xml_diff>
--- a/prototipo_pcr/inputs/produccion_arl.xlsx
+++ b/prototipo_pcr/inputs/produccion_arl.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebatoec/projects/prototipo_pcr/prototipo_pcr/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B55616EB-7C9B-664D-BCD2-26599D0B67EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE6B2B1E-062A-314E-9A8A-6F5D23E852E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="800" windowWidth="28040" windowHeight="17320" xr2:uid="{7D17A6B4-6AD1-1448-967D-6C5E3D1352B8}"/>
   </bookViews>
@@ -503,8 +503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B33A6345-19BA-9347-9343-B7C995C9E91D}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="139" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="139" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -596,8 +596,8 @@
       <c r="J2" s="3">
         <v>45566</v>
       </c>
-      <c r="K2" s="6">
-        <v>202412</v>
+      <c r="K2" s="3">
+        <v>45657</v>
       </c>
       <c r="L2" t="s">
         <v>12</v>
@@ -637,8 +637,8 @@
       <c r="J3" s="3">
         <v>45627</v>
       </c>
-      <c r="K3" s="6">
-        <v>202412</v>
+      <c r="K3" s="3">
+        <v>45657</v>
       </c>
       <c r="L3" t="s">
         <v>12</v>
@@ -678,8 +678,8 @@
       <c r="J4" s="3">
         <v>45658</v>
       </c>
-      <c r="K4" s="6">
-        <v>202412</v>
+      <c r="K4" s="3">
+        <v>45657</v>
       </c>
       <c r="L4" t="s">
         <v>12</v>

</xml_diff>